<commit_message>
Add insert Productionplan to db
</commit_message>
<xml_diff>
--- a/CIM.API/ProductionPlan/test.xlsx
+++ b/CIM.API/ProductionPlan/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSEC\Dole\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB46A3E-E086-4B5B-9DE4-055B2E96A334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1E8BD8-18ED-4FF6-A44E-7579937F2368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{57D68562-AE37-4DA5-A8BD-66CE4E4007B3}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>F</t>
+    <t>J</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +466,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
setup done : ready to coding
</commit_message>
<xml_diff>
--- a/CIM.API/ProductionPlan/test.xlsx
+++ b/CIM.API/ProductionPlan/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSEC\Dole\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\PSEC\Dole\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4403A9BD-8B3C-4F2D-AC9A-F9048183F6C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBB9408-557F-4D36-93F6-D22187414DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{57D68562-AE37-4DA5-A8BD-66CE4E4007B3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F30CFE8-7C2F-4F78-8F9D-70062DE8B2E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,24 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Plant_Id</t>
+    <t>PlantId</t>
   </si>
   <si>
-    <t>Product_Id</t>
+    <t>ProductId</t>
   </si>
   <si>
     <t>Target</t>
   </si>
   <si>
     <t>Unit</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
 </sst>
 </file>
@@ -86,11 +78,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,19 +393,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4008F55-02DD-4D68-8298-B90EFDE140A2}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9BB78E-3A67-4D83-BAD4-5A5348E87064}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,88 +416,74 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>71</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>79</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>33</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>34</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>14</v>
+      <c r="C5">
+        <v>39</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>35</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>50</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>60</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
origin : develop 2020-03-14 : ready to develop
</commit_message>
<xml_diff>
--- a/CIM.API/ProductionPlan/test.xlsx
+++ b/CIM.API/ProductionPlan/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\PSEC\Dole\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSEC\Dole\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBB9408-557F-4D36-93F6-D22187414DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4403A9BD-8B3C-4F2D-AC9A-F9048183F6C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F30CFE8-7C2F-4F78-8F9D-70062DE8B2E5}"/>
+    <workbookView xWindow="7200" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{57D68562-AE37-4DA5-A8BD-66CE4E4007B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,18 +33,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
-    <t>PlantId</t>
+    <t>Plant_Id</t>
   </si>
   <si>
-    <t>ProductId</t>
+    <t>Product_Id</t>
   </si>
   <si>
     <t>Target</t>
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -78,8 +86,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,16 +404,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9BB78E-3A67-4D83-BAD4-5A5348E87064}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4008F55-02DD-4D68-8298-B90EFDE140A2}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,74 +430,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>71</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>42</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>77</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>41</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>78</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>79</v>
-      </c>
-      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>39</v>
+      <c r="C5" s="1">
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>75</v>
-      </c>
-      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>38</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
+      <c r="C7" s="1">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add response model to product api
</commit_message>
<xml_diff>
--- a/CIM.API/ProductionPlan/test.xlsx
+++ b/CIM.API/ProductionPlan/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSEC\Dole\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\PSEC\Dole\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4403A9BD-8B3C-4F2D-AC9A-F9048183F6C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBB9408-557F-4D36-93F6-D22187414DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1815" windowWidth="21600" windowHeight="11385" xr2:uid="{57D68562-AE37-4DA5-A8BD-66CE4E4007B3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F30CFE8-7C2F-4F78-8F9D-70062DE8B2E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,24 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Plant_Id</t>
+    <t>PlantId</t>
   </si>
   <si>
-    <t>Product_Id</t>
+    <t>ProductId</t>
   </si>
   <si>
     <t>Target</t>
   </si>
   <si>
     <t>Unit</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
 </sst>
 </file>
@@ -86,11 +78,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,19 +393,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4008F55-02DD-4D68-8298-B90EFDE140A2}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9BB78E-3A67-4D83-BAD4-5A5348E87064}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,88 +416,74 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>71</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>79</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>33</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>34</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>14</v>
+      <c r="C5">
+        <v>39</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>35</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>50</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>60</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>